<commit_message>
Modified to use one axis
</commit_message>
<xml_diff>
--- a/Songs/Lost Woods to G-Code.xlsx
+++ b/Songs/Lost Woods to G-Code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\Documents\Instructables and Projects\Ender 3 Music\Musical Marlin\Songs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3598A52D-AD85-4193-BFAF-983D7D46D202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14B39F0-9605-484C-A861-F62BA0228510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G-Code Generator" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,12 +474,6 @@
       <color rgb="FF202122"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -579,6 +573,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -627,13 +628,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D10:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,47 +972,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="F4" s="8" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="F4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24">
         <v>120</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="25"/>
       <c r="F5" s="4" t="str">
         <f>_xlfn.CONCAT("G17 \nM350 X1 Y1 \nG91 ","\n",E8,"\n",E9,"\n",E10,"\n",E11,"\n",E12,"\n",E13,"\n",E14,"\n",E15,"\n",E16,"\n",E17,"\n",E18,"\n",E19,"\n",E20,"\n",E21,"\n",E22,"\n",E23,"\n",E24,"\n",E25,"\n",E26,"\n",E27,"\n",E28,"\n",E29,"\n",E30,"\n",E31,"\n",E32,"\n",E33,"\n",E34,"\n",E35,"\n",E36,"\n",E37,"\n",E38,"\n",E39,"\n",E40,"\n",E41,"\n",E42,"\n",E43,"\n",E44,"\n",E45,"\n",E46,"\n",E47,"\n",E48,"\n",E49,"\n",E50)</f>
-        <v>G17 \nM350 X1 Y1 \nG91 \nG0 X0.916666666666667 Y0.916666666666667 F220\nG0 X1.375 Y1.375 F330\nG0 X3.08333333333333 Y3.08333333333333 F370\nG0 X0.916666666666667 Y0.916666666666667 F220\nG0 X1.375 Y1.375 F330\nG0 X3.08333333333333 Y3.08333333333333 F370\nG0 X1.09166666666667 Y1.09166666666667 F262\nG0 X1.375 Y1.375 F330\nG0 X1.54166666666667 Y1.54166666666667 F370\nG0 X2.05833333333333 Y2.05833333333333 F494\nG0 X3.66666666666667 Y3.66666666666667 F440\nG0 X1.54166666666667 Y1.54166666666667 F370\nG0 X1.63333333333333 Y1.63333333333333 F392\nG0 X1.54166666666667 Y1.54166666666667 F370\nG0 X1.225 Y1.225 F294\nG0 X4.11666666666667 Y4.11666666666667 F247\nG0 X0.0625 Y0.0625 F15\nG0 X0.916666666666667 Y0.916666666666667 F220\nG0 X1.02916666666667 Y1.02916666666667 F247\nG0 X1.225 Y1.225 F294\nG0 X6.175 Y6.175 F247\nG0 X1.09166666666667 Y1.09166666666667 F262\nG0 X1.375 Y1.375 F330\nG0 X3.08333333333333 Y3.08333333333333 F370\nG0 X1.09166666666667 Y1.09166666666667 F262\nG0 X1.375 Y1.375 F330\nG0 X3.08333333333333 Y3.08333333333333 F370\nG0 X1.09166666666667 Y1.09166666666667 F262\nG0 X1.375 Y1.375 F330\nG0 X1.54166666666667 Y1.54166666666667 F370\nG0 X2.05833333333333 Y2.05833333333333 F494\nG0 X3.66666666666667 Y3.66666666666667 F440\nG0 X1.54166666666667 Y1.54166666666667 F370\nG0 X1.63333333333333 Y1.63333333333333 F392\nG0 X2.05833333333333 Y2.05833333333333 F494\nG0 X1.54166666666667 Y1.54166666666667 F370\nG0 X4.9 Y4.9 F294\nG0 X0.0625 Y0.0625 F15\nG0 X1.54166666666667 Y1.54166666666667 F370\nG0 X1.225 Y1.225 F294\nG0 X0.916666666666667 Y0.916666666666667 F220\nG0 X6.175 Y6.175 F247\nG0 X0.916666666666667 Y0.916666666666667 F220</v>
+        <v>G17 \nM350 X1 Y1 \nG91 \nG0 X0.916666666666667 F220\nG0 X1.375 F330\nG0 X3.08333333333333 F370\nG0 X0.916666666666667 F220\nG0 X1.375 F330\nG0 X3.08333333333333 F370\nG0 X1.09166666666667 F262\nG0 X1.375 F330\nG0 X1.54166666666667 F370\nG0 X2.05833333333333 F494\nG0 X3.66666666666667 F440\nG0 X1.54166666666667 F370\nG0 X1.63333333333333 F392\nG0 X1.54166666666667 F370\nG0 X1.225 F294\nG0 X4.11666666666667 F247\nG0 X0.0625 F15\nG0 X0.916666666666667 F220\nG0 X1.02916666666667 F247\nG0 X1.225 F294\nG0 X6.175 F247\nG0 X1.09166666666667 F262\nG0 X1.375 F330\nG0 X3.08333333333333 F370\nG0 X1.09166666666667 F262\nG0 X1.375 F330\nG0 X3.08333333333333 F370\nG0 X1.09166666666667 F262\nG0 X1.375 F330\nG0 X1.54166666666667 F370\nG0 X2.05833333333333 F494\nG0 X3.66666666666667 F440\nG0 X1.54166666666667 F370\nG0 X1.63333333333333 F392\nG0 X2.05833333333333 F494\nG0 X1.54166666666667 F370\nG0 X4.9 F294\nG0 X0.0625 F15\nG0 X1.54166666666667 F370\nG0 X1.225 F294\nG0 X0.916666666666667 F220\nG0 X6.175 F247\nG0 X0.916666666666667 F220</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -1057,8 +1051,8 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E8" t="str">
-        <f>_xlfn.CONCAT("G0 X",D8, " Y",D8, " F", B8)</f>
-        <v>G0 X0.916666666666667 Y0.916666666666667 F220</v>
+        <f>_xlfn.CONCAT("G0 X",D8, " F", B8)</f>
+        <v>G0 X0.916666666666667 F220</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1077,8 +1071,8 @@
         <v>1.375</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ref="E9:E58" si="1">_xlfn.CONCAT("G0 X",D9, " Y",D9, " F", B9)</f>
-        <v>G0 X1.375 Y1.375 F330</v>
+        <f t="shared" ref="E9:E58" si="1">_xlfn.CONCAT("G0 X",D9, " F", B9)</f>
+        <v>G0 X1.375 F330</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1098,7 +1092,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X3.08333333333333 Y3.08333333333333 F370</v>
+        <v>G0 X3.08333333333333 F370</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1118,7 +1112,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X0.916666666666667 Y0.916666666666667 F220</v>
+        <v>G0 X0.916666666666667 F220</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1138,7 +1132,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.375 Y1.375 F330</v>
+        <v>G0 X1.375 F330</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1158,7 +1152,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X3.08333333333333 Y3.08333333333333 F370</v>
+        <v>G0 X3.08333333333333 F370</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1178,7 +1172,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.09166666666667 Y1.09166666666667 F262</v>
+        <v>G0 X1.09166666666667 F262</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1198,7 +1192,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.375 Y1.375 F330</v>
+        <v>G0 X1.375 F330</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1218,7 +1212,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.54166666666667 Y1.54166666666667 F370</v>
+        <v>G0 X1.54166666666667 F370</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,7 +1232,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X2.05833333333333 Y2.05833333333333 F494</v>
+        <v>G0 X2.05833333333333 F494</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1258,7 +1252,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X3.66666666666667 Y3.66666666666667 F440</v>
+        <v>G0 X3.66666666666667 F440</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,7 +1272,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.54166666666667 Y1.54166666666667 F370</v>
+        <v>G0 X1.54166666666667 F370</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,7 +1292,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.63333333333333 Y1.63333333333333 F392</v>
+        <v>G0 X1.63333333333333 F392</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1318,7 +1312,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.54166666666667 Y1.54166666666667 F370</v>
+        <v>G0 X1.54166666666667 F370</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1338,7 +1332,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.225 Y1.225 F294</v>
+        <v>G0 X1.225 F294</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,7 +1352,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X4.11666666666667 Y4.11666666666667 F247</v>
+        <v>G0 X4.11666666666667 F247</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1372,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X0.0625 Y0.0625 F15</v>
+        <v>G0 X0.0625 F15</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,7 +1392,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X0.916666666666667 Y0.916666666666667 F220</v>
+        <v>G0 X0.916666666666667 F220</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,7 +1412,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.02916666666667 Y1.02916666666667 F247</v>
+        <v>G0 X1.02916666666667 F247</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,7 +1432,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.225 Y1.225 F294</v>
+        <v>G0 X1.225 F294</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1458,7 +1452,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X6.175 Y6.175 F247</v>
+        <v>G0 X6.175 F247</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1478,7 +1472,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.09166666666667 Y1.09166666666667 F262</v>
+        <v>G0 X1.09166666666667 F262</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,7 +1492,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.375 Y1.375 F330</v>
+        <v>G0 X1.375 F330</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,7 +1512,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X3.08333333333333 Y3.08333333333333 F370</v>
+        <v>G0 X3.08333333333333 F370</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,7 +1532,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.09166666666667 Y1.09166666666667 F262</v>
+        <v>G0 X1.09166666666667 F262</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,7 +1552,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.375 Y1.375 F330</v>
+        <v>G0 X1.375 F330</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1578,7 +1572,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X3.08333333333333 Y3.08333333333333 F370</v>
+        <v>G0 X3.08333333333333 F370</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,7 +1592,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.09166666666667 Y1.09166666666667 F262</v>
+        <v>G0 X1.09166666666667 F262</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1618,7 +1612,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.375 Y1.375 F330</v>
+        <v>G0 X1.375 F330</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1638,7 +1632,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.54166666666667 Y1.54166666666667 F370</v>
+        <v>G0 X1.54166666666667 F370</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,7 +1652,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X2.05833333333333 Y2.05833333333333 F494</v>
+        <v>G0 X2.05833333333333 F494</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1678,7 +1672,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X3.66666666666667 Y3.66666666666667 F440</v>
+        <v>G0 X3.66666666666667 F440</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,12 +1687,12 @@
         <v>0.5</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" ref="D40:D71" si="2">(1/$C$5)*C40*B40</f>
+        <f t="shared" ref="D40:D58" si="2">(1/$C$5)*C40*B40</f>
         <v>1.5416666666666667</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.54166666666667 Y1.54166666666667 F370</v>
+        <v>G0 X1.54166666666667 F370</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1718,7 +1712,7 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.63333333333333 Y1.63333333333333 F392</v>
+        <v>G0 X1.63333333333333 F392</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1738,7 +1732,7 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X2.05833333333333 Y2.05833333333333 F494</v>
+        <v>G0 X2.05833333333333 F494</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1758,7 +1752,7 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.54166666666667 Y1.54166666666667 F370</v>
+        <v>G0 X1.54166666666667 F370</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1778,7 +1772,7 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X4.9 Y4.9 F294</v>
+        <v>G0 X4.9 F294</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1798,7 +1792,7 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X0.0625 Y0.0625 F15</v>
+        <v>G0 X0.0625 F15</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,7 +1812,7 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.54166666666667 Y1.54166666666667 F370</v>
+        <v>G0 X1.54166666666667 F370</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1838,7 +1832,7 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.225 Y1.225 F294</v>
+        <v>G0 X1.225 F294</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,7 +1852,7 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X0.916666666666667 Y0.916666666666667 F220</v>
+        <v>G0 X0.916666666666667 F220</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1878,7 +1872,7 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X6.175 Y6.175 F247</v>
+        <v>G0 X6.175 F247</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,7 +1892,7 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X0.916666666666667 Y0.916666666666667 F220</v>
+        <v>G0 X0.916666666666667 F220</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1918,7 +1912,7 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.02916666666667 Y1.02916666666667 F247</v>
+        <v>G0 X1.02916666666667 F247</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,7 +1932,7 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X2.18333333333333 Y2.18333333333333 F262</v>
+        <v>G0 X2.18333333333333 F262</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1958,7 +1952,7 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.225 Y1.225 F294</v>
+        <v>G0 X1.225 F294</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,7 +1972,7 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.375 Y1.375 F330</v>
+        <v>G0 X1.375 F330</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1998,7 +1992,7 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X3.08333333333333 Y3.08333333333333 F370</v>
+        <v>G0 X3.08333333333333 F370</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2018,7 +2012,7 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.63333333333333 Y1.63333333333333 F392</v>
+        <v>G0 X1.63333333333333 F392</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2038,7 +2032,7 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X1.83333333333333 Y1.83333333333333 F440</v>
+        <v>G0 X1.83333333333333 F440</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,7 +2052,7 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
-        <v>G0 X6.175 Y6.175 F247</v>
+        <v>G0 X6.175 F247</v>
       </c>
     </row>
   </sheetData>
@@ -2080,7 +2074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBC0FE0-A112-4E23-88F9-6147D2961CB6}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -2093,38 +2087,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22">
+      <c r="B5" s="29"/>
+      <c r="C5" s="29">
         <v>80</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2141,145 +2135,145 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="9">
         <v>1046.502</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="8">
         <f>(B8*60)/$C$5</f>
         <v>784.87649999999996</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="8">
         <f>ROUND(C8,0)</f>
         <v>785</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="9">
         <v>987.76660000000004</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="8">
         <f t="shared" ref="C9:C58" si="0">(B9*60)/$C$5</f>
         <v>740.82494999999994</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="8">
         <f t="shared" ref="D9:D58" si="1">ROUND(C9,0)</f>
         <v>741</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="9">
         <v>932.32749999999999</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>699.24562500000002</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="8">
         <f t="shared" si="1"/>
         <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="10">
         <v>880</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="8">
         <f t="shared" si="0"/>
         <v>660</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="8">
         <f t="shared" si="1"/>
         <v>660</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="9">
         <v>830.60940000000005</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="8">
         <f t="shared" si="0"/>
         <v>622.95705000000009</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="8">
         <f t="shared" si="1"/>
         <v>623</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="9">
         <v>783.99090000000001</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="8">
         <f t="shared" si="0"/>
         <v>587.99317499999995</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="8">
         <f t="shared" si="1"/>
         <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="9">
         <v>739.98879999999997</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="8">
         <f t="shared" si="0"/>
         <v>554.99160000000006</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="8">
         <f t="shared" si="1"/>
         <v>555</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="9">
         <v>698.45650000000001</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="8">
         <f t="shared" si="0"/>
         <v>523.84237499999995</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="8">
         <f t="shared" si="1"/>
         <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="9">
         <v>659.25509999999997</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="8">
         <f t="shared" si="0"/>
         <v>494.44132499999995</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="8">
         <f t="shared" si="1"/>
         <v>494</v>
       </c>
@@ -2288,7 +2282,7 @@
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="11">
         <v>622.25400000000002</v>
       </c>
       <c r="C17">
@@ -2304,7 +2298,7 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="11">
         <v>587.32950000000005</v>
       </c>
       <c r="C18">
@@ -2320,7 +2314,7 @@
       <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="11">
         <v>554.36530000000005</v>
       </c>
       <c r="C19">
@@ -2336,7 +2330,7 @@
       <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="11">
         <v>523.25109999999995</v>
       </c>
       <c r="C20">
@@ -2352,7 +2346,7 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="11">
         <v>493.88330000000002</v>
       </c>
       <c r="C21">
@@ -2368,7 +2362,7 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="11">
         <v>466.16379999999998</v>
       </c>
       <c r="C22">
@@ -2384,7 +2378,7 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="12">
         <v>440</v>
       </c>
       <c r="C23">
@@ -2400,7 +2394,7 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="11">
         <v>415.30470000000003</v>
       </c>
       <c r="C24">
@@ -2416,7 +2410,7 @@
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="11">
         <v>391.99540000000002</v>
       </c>
       <c r="C25">
@@ -2432,7 +2426,7 @@
       <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="11">
         <v>369.99439999999998</v>
       </c>
       <c r="C26">
@@ -2448,7 +2442,7 @@
       <c r="A27" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="11">
         <v>349.22820000000002</v>
       </c>
       <c r="C27">
@@ -2464,7 +2458,7 @@
       <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="11">
         <v>329.62759999999997</v>
       </c>
       <c r="C28">
@@ -2480,7 +2474,7 @@
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="11">
         <v>311.12700000000001</v>
       </c>
       <c r="C29">
@@ -2496,7 +2490,7 @@
       <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="11">
         <v>293.66480000000001</v>
       </c>
       <c r="C30">
@@ -2512,7 +2506,7 @@
       <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="11">
         <v>277.18259999999998</v>
       </c>
       <c r="C31">
@@ -2528,7 +2522,7 @@
       <c r="A32" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="29">
+      <c r="B32" s="13">
         <v>261.62560000000002</v>
       </c>
       <c r="C32">
@@ -2544,7 +2538,7 @@
       <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="11">
         <v>246.9417</v>
       </c>
       <c r="C33">
@@ -2560,7 +2554,7 @@
       <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B34" s="11">
         <v>233.08189999999999</v>
       </c>
       <c r="C34">
@@ -2576,7 +2570,7 @@
       <c r="A35" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="14">
         <v>220</v>
       </c>
       <c r="C35">
@@ -2592,7 +2586,7 @@
       <c r="A36" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="11">
         <v>207.6523</v>
       </c>
       <c r="C36">
@@ -2608,7 +2602,7 @@
       <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="11">
         <v>195.99770000000001</v>
       </c>
       <c r="C37">
@@ -2624,7 +2618,7 @@
       <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="11">
         <v>184.99719999999999</v>
       </c>
       <c r="C38">
@@ -2640,7 +2634,7 @@
       <c r="A39" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B39" s="11">
         <v>174.61410000000001</v>
       </c>
       <c r="C39">
@@ -2656,7 +2650,7 @@
       <c r="A40" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="27">
+      <c r="B40" s="11">
         <v>164.81379999999999</v>
       </c>
       <c r="C40">
@@ -2672,7 +2666,7 @@
       <c r="A41" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="27">
+      <c r="B41" s="11">
         <v>155.5635</v>
       </c>
       <c r="C41">
@@ -2688,7 +2682,7 @@
       <c r="A42" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="27">
+      <c r="B42" s="11">
         <v>146.83240000000001</v>
       </c>
       <c r="C42">
@@ -2704,7 +2698,7 @@
       <c r="A43" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="27">
+      <c r="B43" s="11">
         <v>138.59129999999999</v>
       </c>
       <c r="C43">
@@ -2720,7 +2714,7 @@
       <c r="A44" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="27">
+      <c r="B44" s="11">
         <v>130.81280000000001</v>
       </c>
       <c r="C44">
@@ -2736,7 +2730,7 @@
       <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B45" s="11">
         <v>123.4708</v>
       </c>
       <c r="C45">
@@ -2752,7 +2746,7 @@
       <c r="A46" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="27">
+      <c r="B46" s="11">
         <v>116.54089999999999</v>
       </c>
       <c r="C46">
@@ -2768,7 +2762,7 @@
       <c r="A47" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="30">
+      <c r="B47" s="14">
         <v>110</v>
       </c>
       <c r="C47">
@@ -2784,7 +2778,7 @@
       <c r="A48" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="27">
+      <c r="B48" s="11">
         <v>103.8262</v>
       </c>
       <c r="C48">
@@ -2800,7 +2794,7 @@
       <c r="A49" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="27">
+      <c r="B49" s="11">
         <v>97.998859999999993</v>
       </c>
       <c r="C49">
@@ -2816,7 +2810,7 @@
       <c r="A50" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="27">
+      <c r="B50" s="11">
         <v>92.498609999999999</v>
       </c>
       <c r="C50">
@@ -2832,7 +2826,7 @@
       <c r="A51" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="27">
+      <c r="B51" s="11">
         <v>87.307060000000007</v>
       </c>
       <c r="C51">
@@ -2848,7 +2842,7 @@
       <c r="A52" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="27">
+      <c r="B52" s="11">
         <v>82.406890000000004</v>
       </c>
       <c r="C52">
@@ -2864,7 +2858,7 @@
       <c r="A53" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="27">
+      <c r="B53" s="11">
         <v>77.781750000000002</v>
       </c>
       <c r="C53">
@@ -2880,7 +2874,7 @@
       <c r="A54" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="27">
+      <c r="B54" s="11">
         <v>73.41619</v>
       </c>
       <c r="C54">
@@ -2896,7 +2890,7 @@
       <c r="A55" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="27">
+      <c r="B55" s="11">
         <v>69.295659999999998</v>
       </c>
       <c r="C55">
@@ -2912,7 +2906,7 @@
       <c r="A56" t="s">
         <v>65</v>
       </c>
-      <c r="B56" s="27">
+      <c r="B56" s="11">
         <v>65.406390000000002</v>
       </c>
       <c r="C56">
@@ -2928,7 +2922,7 @@
       <c r="A58" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="27">
+      <c r="B58" s="11">
         <v>20</v>
       </c>
       <c r="C58">

</xml_diff>